<commit_message>
Planilha de requisitas avançada(Víctor Vicente)
Tabela de requisitos com o que eu achei do tamanho e ordem de execução
</commit_message>
<xml_diff>
--- a/Análise de requisitos.xlsx
+++ b/Análise de requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\BandTec\Tecnologia da Informação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\HTML yoshi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF071B6C-B762-4660-B1FF-21DF084FC4AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807C999-6801-42F5-B349-DD52DA204120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2682398-801E-4576-ADD2-A3BB594430BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>Requisitos</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Histórico de temperatura da geladeira</t>
+  </si>
+  <si>
+    <t>Tamanho</t>
+  </si>
+  <si>
+    <t>Ordem de execução</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -237,15 +246,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -279,18 +297,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:D21" xr:uid="{E5CEC0B4-FB5D-43A4-87CD-1CF95FD20E67}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:F21" xr:uid="{E5CEC0B4-FB5D-43A4-87CD-1CF95FD20E67}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="0"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
+    <sortCondition ref="F8"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{5119A67A-FDA7-4314-B098-FA33C7F5B6DA}" name="Requisitos"/>
     <tableColumn id="3" xr3:uid="{8C3F0BD9-833A-447B-8627-C63D0CA20106}" name="Classificação"/>
     <tableColumn id="4" xr3:uid="{56A0A581-29CD-4319-AC8F-344112829072}" name="Funicional/Não funcinal"/>
+    <tableColumn id="5" xr3:uid="{AA5ABCD9-3517-458A-BC1C-DC30EDC7EC32}" name="Tamanho" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FF99333B-30EC-4E02-B88F-15C59A660E08}" name="Ordem de execução" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -593,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEA6CB8-8AFC-41CE-AAFA-438A394CFF4E}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,10 +629,12 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -620,13 +647,19 @@
       <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -634,27 +667,39 @@
       <c r="D2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E3" s="3">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -662,97 +707,139 @@
       <c r="D4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E10" s="3">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
@@ -760,55 +847,79 @@
       <c r="D11" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>15</v>
       </c>
-      <c r="D13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
       <c r="D14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3">
+        <v>21</v>
+      </c>
+      <c r="F14" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -816,89 +927,131 @@
       <c r="D15" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="3">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>15</v>
-      </c>
       <c r="D19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Análise individual de requisitos
Análise de Henrique sobre a sprint
</commit_message>
<xml_diff>
--- a/Análise de requisitos.xlsx
+++ b/Análise de requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\HTML yoshi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807C999-6801-42F5-B349-DD52DA204120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D25B1DA-6FEF-4A7D-AFDA-7C2A051D74B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2682398-801E-4576-ADD2-A3BB594430BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>Requisitos</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Aviso de "vencimento" de produto para a empresa</t>
   </si>
   <si>
-    <t>Envio de informações em tempo real</t>
-  </si>
-  <si>
     <t>Funicional/Não funcinal</t>
   </si>
   <si>
@@ -186,10 +183,13 @@
     <t>Tamanho</t>
   </si>
   <si>
-    <t>Ordem de execução</t>
-  </si>
-  <si>
-    <t>#</t>
+    <t>Ordem de exec.</t>
+  </si>
+  <si>
+    <t>Envio de informações online</t>
+  </si>
+  <si>
+    <t>NÃO</t>
   </si>
 </sst>
 </file>
@@ -246,23 +246,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -297,7 +291,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:F21" xr:uid="{E5CEC0B4-FB5D-43A4-87CD-1CF95FD20E67}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -306,16 +300,15 @@
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
-    <sortCondition ref="F8"/>
-  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{5119A67A-FDA7-4314-B098-FA33C7F5B6DA}" name="Requisitos"/>
     <tableColumn id="3" xr3:uid="{8C3F0BD9-833A-447B-8627-C63D0CA20106}" name="Classificação"/>
     <tableColumn id="4" xr3:uid="{56A0A581-29CD-4319-AC8F-344112829072}" name="Funicional/Não funcinal"/>
-    <tableColumn id="5" xr3:uid="{AA5ABCD9-3517-458A-BC1C-DC30EDC7EC32}" name="Tamanho" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{FF99333B-30EC-4E02-B88F-15C59A660E08}" name="Ordem de execução" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{5C74AC34-A030-4017-B8AF-AAC6F18158CE}" name="Tamanho" dataDxfId="0">
+      <calculatedColumnFormula>----B6i</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{9A29EA30-7F4F-46BE-8D2D-0F09735CABB1}" name="Ordem de exec."/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,7 +614,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,9 +622,9 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -645,181 +638,169 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="3">
+        <v>45</v>
+      </c>
+      <c r="E2">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
-        <v>1</v>
+      <c r="F2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="3">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3">
-        <v>2</v>
+      <c r="E3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="3">
-        <v>8</v>
-      </c>
-      <c r="F4" s="3">
-        <v>3</v>
+        <v>45</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="3">
-        <v>5</v>
-      </c>
-      <c r="F5" s="3">
-        <v>4</v>
+      <c r="E5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="3">
-        <v>8</v>
-      </c>
-      <c r="F6" s="3">
-        <v>5</v>
+      <c r="E6" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="3">
-        <v>5</v>
-      </c>
-      <c r="F7" s="3">
-        <v>6</v>
+        <v>45</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="3">
-        <v>3</v>
-      </c>
-      <c r="F8" s="3">
-        <v>7</v>
+      <c r="E8" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" s="3">
-        <v>3</v>
-      </c>
-      <c r="F9" s="3">
-        <v>8</v>
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -827,231 +808,225 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="3">
-        <v>13</v>
-      </c>
-      <c r="F10" s="3">
-        <v>9</v>
+      <c r="E10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="3">
-        <v>13</v>
-      </c>
-      <c r="F11" s="3">
-        <v>10</v>
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="3">
-        <v>5</v>
-      </c>
-      <c r="F12" s="3">
-        <v>11</v>
+      <c r="E12">
+        <v>21</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="3">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3">
-        <v>12</v>
+        <v>45</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="3">
-        <v>21</v>
-      </c>
-      <c r="F14" s="3">
+        <v>45</v>
+      </c>
+      <c r="E14">
         <v>13</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="3">
-        <v>21</v>
-      </c>
-      <c r="F15" s="3">
-        <v>14</v>
+        <v>45</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
+      </c>
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21">
+        <v>13</v>
+      </c>
+      <c r="F21">
         <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabela de requisitos avançados (Víctor Vicente)
Minha tabela de requisitos sobre o que eu acho do tamanho e a ordem de execução.
</commit_message>
<xml_diff>
--- a/Análise de requisitos.xlsx
+++ b/Análise de requisitos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Documents\HTML yoshi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D25B1DA-6FEF-4A7D-AFDA-7C2A051D74B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A807C999-6801-42F5-B349-DD52DA204120}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2682398-801E-4576-ADD2-A3BB594430BC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>Requisitos</t>
   </si>
@@ -162,6 +162,9 @@
     <t>Aviso de "vencimento" de produto para a empresa</t>
   </si>
   <si>
+    <t>Envio de informações em tempo real</t>
+  </si>
+  <si>
     <t>Funicional/Não funcinal</t>
   </si>
   <si>
@@ -183,13 +186,10 @@
     <t>Tamanho</t>
   </si>
   <si>
-    <t>Ordem de exec.</t>
-  </si>
-  <si>
-    <t>Envio de informações online</t>
-  </si>
-  <si>
-    <t>NÃO</t>
+    <t>Ordem de execução</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -246,17 +246,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -291,7 +297,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{82E0990A-4B9A-4F13-ACA4-EF4F95E68100}" name="Tabela1" displayName="Tabela1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:F21" xr:uid="{E5CEC0B4-FB5D-43A4-87CD-1CF95FD20E67}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -300,15 +306,16 @@
     <filterColumn colId="4" hiddenButton="1"/>
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
+    <sortCondition ref="F8"/>
+  </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{100ECBF8-63E0-440C-9397-9E6AABD71A85}" name="ID" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{5119A67A-FDA7-4314-B098-FA33C7F5B6DA}" name="Requisitos"/>
     <tableColumn id="3" xr3:uid="{8C3F0BD9-833A-447B-8627-C63D0CA20106}" name="Classificação"/>
     <tableColumn id="4" xr3:uid="{56A0A581-29CD-4319-AC8F-344112829072}" name="Funicional/Não funcinal"/>
-    <tableColumn id="5" xr3:uid="{5C74AC34-A030-4017-B8AF-AAC6F18158CE}" name="Tamanho" dataDxfId="0">
-      <calculatedColumnFormula>----B6i</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{9A29EA30-7F4F-46BE-8D2D-0F09735CABB1}" name="Ordem de exec."/>
+    <tableColumn id="5" xr3:uid="{AA5ABCD9-3517-458A-BC1C-DC30EDC7EC32}" name="Tamanho" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FF99333B-30EC-4E02-B88F-15C59A660E08}" name="Ordem de execução" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -614,7 +621,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,9 +629,9 @@
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -638,169 +645,181 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2">
+        <v>46</v>
+      </c>
+      <c r="E2" s="3">
         <v>13</v>
       </c>
-      <c r="F2">
-        <v>5</v>
+      <c r="F2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" t="s">
-        <v>51</v>
+      <c r="E3" s="3">
+        <v>21</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>21</v>
-      </c>
-      <c r="F4">
-        <v>6</v>
+        <v>46</v>
+      </c>
+      <c r="E4" s="3">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" t="s">
-        <v>51</v>
+      <c r="E5" s="3">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" t="s">
-        <v>51</v>
+      <c r="F6" s="3">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="E7" s="3">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
+      <c r="E8" s="3">
+        <v>3</v>
+      </c>
+      <c r="F8" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
+        <v>3</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -808,225 +827,231 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
-        <v>51</v>
+      <c r="E10" s="3">
+        <v>13</v>
+      </c>
+      <c r="F10" s="3">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11">
-        <v>8</v>
-      </c>
-      <c r="F11">
-        <v>11</v>
+        <v>46</v>
+      </c>
+      <c r="E11" s="3">
+        <v>13</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="E12">
-        <v>21</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
+      <c r="E12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13">
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>8</v>
+        <v>46</v>
+      </c>
+      <c r="E13" s="3">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14">
+        <v>46</v>
+      </c>
+      <c r="E14" s="3">
+        <v>21</v>
+      </c>
+      <c r="F14" s="3">
         <v>13</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
+        <v>46</v>
+      </c>
+      <c r="E15" s="3">
+        <v>21</v>
+      </c>
+      <c r="F15" s="3">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>7</v>
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20">
-        <v>13</v>
-      </c>
-      <c r="F20">
-        <v>14</v>
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21">
-        <v>13</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
+        <v>47</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>